<commit_message>
updated the status tracker with this week's final values and estimates for the next week
</commit_message>
<xml_diff>
--- a/docs/StatusTracker_week4.xlsx
+++ b/docs/StatusTracker_week4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\SG2PEPF000126DE\EXCELCNV\1cfc5f48-be4e-4c83-ae59-8ee1f65fc805\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinitmehta/Desktop/IIITH/Sem4/DASS/Project/dass-project-spring-2024-team-41/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{882BAED9-1FD7-477D-AB6A-03F31C292623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FF95CB-C048-5D4C-90D6-B0C4BBEBF97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -446,7 +446,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -596,85 +596,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1134,78 +1056,78 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="C2" s="17"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30.95" customHeight="1">
+    <row r="19" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="26.1" customHeight="1">
+    <row r="20" spans="1:2" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>14</v>
       </c>
@@ -1221,7 +1143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="26.1" customHeight="1">
+    <row r="21" spans="1:2" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>16</v>
       </c>
@@ -1229,7 +1151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="38.1" customHeight="1">
+    <row r="22" spans="1:2" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>18</v>
       </c>
@@ -1237,27 +1159,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18">
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18">
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18">
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B25" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18">
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18">
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B27" s="19"/>
     </row>
   </sheetData>
@@ -1272,23 +1194,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="93.42578125" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="93.5" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.95" customHeight="1">
+    <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="str">
         <f>(Instructions!A19)</f>
         <v>PROJECT NUMBER</v>
@@ -1297,7 +1219,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="26.1" customHeight="1">
+    <row r="2" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22" t="str">
         <f>(Instructions!A20)</f>
         <v>PROJECT NAME</v>
@@ -1306,7 +1228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.95" customHeight="1">
+    <row r="3" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="str">
         <f>(Instructions!A21)</f>
         <v>PROJECT MENTOR (sponsor)</v>
@@ -1315,7 +1237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="9" customFormat="1" ht="38.25">
+    <row r="5" spans="1:9" s="9" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
@@ -1344,7 +1266,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" outlineLevel="2">
+    <row r="6" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1363,7 +1285,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:9" outlineLevel="2">
+    <row r="7" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1391,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" outlineLevel="2">
+    <row r="8" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1419,7 +1341,7 @@
         <v>199.99999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:9" outlineLevel="2">
+    <row r="9" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>41</v>
       </c>
@@ -1450,7 +1372,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.1" customHeight="1" outlineLevel="2">
+    <row r="10" spans="1:9" ht="14" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>44</v>
       </c>
@@ -1481,7 +1403,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" outlineLevel="2">
+    <row r="11" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>46</v>
       </c>
@@ -1512,7 +1434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="24" outlineLevel="2">
+    <row r="12" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1540,7 +1462,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:9" outlineLevel="2">
+    <row r="13" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1568,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" outlineLevel="2">
+    <row r="14" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1596,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" outlineLevel="2">
+    <row r="15" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -1613,7 +1535,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" outlineLevel="2">
+    <row r="16" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1638,7 +1560,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" outlineLevel="2">
+    <row r="17" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1663,7 +1585,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="25.5" outlineLevel="2">
+    <row r="18" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>56</v>
       </c>
@@ -1694,7 +1616,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="19" spans="1:9" outlineLevel="2">
+    <row r="19" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>58</v>
       </c>
@@ -1725,7 +1647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" outlineLevel="2">
+    <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1750,7 +1672,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" outlineLevel="2">
+    <row r="21" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1779,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1804,7 +1726,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1832,7 +1754,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" outlineLevel="2">
+    <row r="24" spans="1:9" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -1849,7 +1771,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1880,7 +1802,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1908,7 +1830,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1939,7 +1861,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -1970,7 +1892,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -2001,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2032,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2060,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -2091,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -2110,7 +2032,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2138,7 +2060,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -2166,7 +2088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2179,19 +2101,22 @@
       <c r="D36" s="5">
         <v>2</v>
       </c>
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
       <c r="F36" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="12" t="str">
+      <c r="H36" s="12">
         <f>IF(OR(D36="", E36=""), "", D36-E36)</f>
-        <v/>
-      </c>
-      <c r="I36" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I36" s="12">
         <f>IF(OR(H36="",E36=0),"",ABS(H36)/E36*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2202,7 +2127,10 @@
         <v>42</v>
       </c>
       <c r="D37" s="5">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="E37" s="5">
+        <v>2</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>55</v>
@@ -2210,16 +2138,16 @@
       <c r="G37" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I37" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="H37" s="12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I37" s="12">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2232,19 +2160,22 @@
       <c r="D38" s="5">
         <v>2</v>
       </c>
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
       <c r="F38" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H38" s="12" t="str">
+      <c r="H38" s="12">
         <f>IF(OR(D38="", E38=""), "", D38-E38)</f>
-        <v/>
-      </c>
-      <c r="I38" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I38" s="12">
         <f>IF(OR(H38="",E38=0),"",ABS(H38)/E38*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2257,19 +2188,22 @@
       <c r="D39" s="5">
         <v>6</v>
       </c>
+      <c r="E39" s="5">
+        <v>2</v>
+      </c>
       <c r="F39" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H39" s="12" t="str">
+      <c r="H39" s="12">
         <f>IF(OR(D39="", E39=""), "", D39-E39)</f>
-        <v/>
-      </c>
-      <c r="I39" s="12" t="str">
+        <v>4</v>
+      </c>
+      <c r="I39" s="12">
         <f>IF(OR(H39="",E39=0),"",ABS(H39)/E39*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -2282,19 +2216,22 @@
       <c r="D40" s="5">
         <v>2</v>
       </c>
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
       <c r="F40" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H40" s="12" t="str">
+      <c r="H40" s="12">
         <f>IF(OR(D40="", E40=""), "", D40-E40)</f>
-        <v/>
-      </c>
-      <c r="I40" s="12" t="str">
+        <v>1</v>
+      </c>
+      <c r="I40" s="12">
         <f>IF(OR(H40="",E40=0),"",ABS(H40)/E40*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -2322,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -2353,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2366,19 +2303,22 @@
       <c r="D43" s="5">
         <v>5</v>
       </c>
+      <c r="E43" s="5">
+        <v>5</v>
+      </c>
       <c r="F43" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H43" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I43" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="H43" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -2397,7 +2337,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2422,7 +2362,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2447,7 +2387,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2472,7 +2412,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -2497,7 +2437,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -2522,7 +2462,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -2547,7 +2487,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H51" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2557,7 +2497,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H52" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2567,7 +2507,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H53" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2577,7 +2517,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H54" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2587,7 +2527,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H55" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2597,7 +2537,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H56" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2607,7 +2547,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H57" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2617,7 +2557,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H58" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2627,7 +2567,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H59" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2637,7 +2577,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H60" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2647,7 +2587,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H61" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2657,7 +2597,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H62" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2667,7 +2607,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H63" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2677,7 +2617,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H64" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2687,7 +2627,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="8:9">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H65" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2697,7 +2637,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="8:9">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H66" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2707,7 +2647,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="8:9">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H67" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2717,7 +2657,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="8:9">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H68" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2727,7 +2667,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="8:9">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H69" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2737,7 +2677,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="8:9">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H70" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2747,7 +2687,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="8:9">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H71" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2757,7 +2697,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="8:9">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H72" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2767,7 +2707,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="8:9">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H73" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2777,7 +2717,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="8:9">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H74" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2787,7 +2727,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="8:9">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H75" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2797,7 +2737,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="8:9">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H76" s="12" t="str">
         <f t="shared" ref="H76:H139" si="2">IF(OR(D76="", E76=""), "", D76-E76)</f>
         <v/>
@@ -2807,7 +2747,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="8:9">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H77" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2817,7 +2757,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="8:9">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H78" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2827,7 +2767,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="8:9">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H79" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2837,7 +2777,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="8:9">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H80" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2847,7 +2787,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="8:9">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H81" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2857,7 +2797,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="8:9">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H82" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2867,7 +2807,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="8:9">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H83" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2877,7 +2817,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="8:9">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H84" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2887,7 +2827,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="8:9">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H85" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2897,7 +2837,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="8:9">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H86" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2907,7 +2847,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="8:9">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H87" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2917,7 +2857,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="8:9">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H88" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2927,7 +2867,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="8:9">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H89" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2937,7 +2877,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="8:9">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H90" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2947,7 +2887,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="8:9">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H91" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2957,7 +2897,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="8:9">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H92" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2967,7 +2907,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="8:9">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H93" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2977,7 +2917,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="8:9">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H94" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2987,7 +2927,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="8:9">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H95" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2997,7 +2937,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="8:9">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H96" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3007,7 +2947,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="8:9">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H97" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3017,7 +2957,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="8:9">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H98" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3027,7 +2967,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="8:9">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H99" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3037,7 +2977,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="8:9">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H100" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3047,7 +2987,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="8:9">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H101" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3057,7 +2997,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="8:9">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H102" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3067,7 +3007,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="8:9">
+    <row r="103" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H103" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3077,7 +3017,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="8:9">
+    <row r="104" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H104" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3087,7 +3027,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="8:9">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H105" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3097,7 +3037,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="8:9">
+    <row r="106" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H106" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3107,7 +3047,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="8:9">
+    <row r="107" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H107" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3117,7 +3057,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="8:9">
+    <row r="108" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H108" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3127,7 +3067,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="8:9">
+    <row r="109" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H109" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3137,7 +3077,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="8:9">
+    <row r="110" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H110" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3147,7 +3087,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="8:9">
+    <row r="111" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H111" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3157,7 +3097,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="8:9">
+    <row r="112" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H112" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3167,7 +3107,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="8:9">
+    <row r="113" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H113" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3177,7 +3117,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="8:9">
+    <row r="114" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H114" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3187,7 +3127,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="8:9">
+    <row r="115" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H115" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3197,7 +3137,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="8:9">
+    <row r="116" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H116" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3207,7 +3147,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="8:9">
+    <row r="117" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H117" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3217,7 +3157,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="8:9">
+    <row r="118" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H118" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3227,7 +3167,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="8:9">
+    <row r="119" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H119" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3237,7 +3177,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="8:9">
+    <row r="120" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H120" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3247,7 +3187,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="8:9">
+    <row r="121" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H121" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3257,7 +3197,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="8:9">
+    <row r="122" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H122" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3267,7 +3207,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="8:9">
+    <row r="123" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H123" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3277,7 +3217,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="8:9">
+    <row r="124" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H124" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3287,7 +3227,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="8:9">
+    <row r="125" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H125" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3297,7 +3237,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="8:9">
+    <row r="126" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H126" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3307,7 +3247,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="8:9">
+    <row r="127" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H127" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3317,7 +3257,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="8:9">
+    <row r="128" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H128" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3327,7 +3267,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="8:9">
+    <row r="129" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H129" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3337,7 +3277,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="8:9">
+    <row r="130" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H130" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3347,7 +3287,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="8:9">
+    <row r="131" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H131" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3357,7 +3297,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="8:9">
+    <row r="132" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H132" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3367,7 +3307,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="8:9">
+    <row r="133" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H133" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3377,7 +3317,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="8:9">
+    <row r="134" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H134" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3387,7 +3327,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="8:9">
+    <row r="135" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H135" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3397,7 +3337,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="8:9">
+    <row r="136" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H136" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3407,7 +3347,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="8:9">
+    <row r="137" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H137" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3417,7 +3357,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="8:9">
+    <row r="138" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H138" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3427,7 +3367,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="8:9">
+    <row r="139" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H139" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3437,7 +3377,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="8:9">
+    <row r="140" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H140" s="12" t="str">
         <f t="shared" ref="H140:H203" si="4">IF(OR(D140="", E140=""), "", D140-E140)</f>
         <v/>
@@ -3447,7 +3387,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="8:9">
+    <row r="141" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H141" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3457,7 +3397,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="8:9">
+    <row r="142" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H142" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3467,7 +3407,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="8:9">
+    <row r="143" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H143" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3477,7 +3417,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="8:9">
+    <row r="144" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H144" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3487,7 +3427,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="8:9">
+    <row r="145" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H145" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3497,7 +3437,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="8:9">
+    <row r="146" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H146" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3507,7 +3447,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="8:9">
+    <row r="147" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H147" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3517,7 +3457,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="8:9">
+    <row r="148" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H148" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3527,7 +3467,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="8:9">
+    <row r="149" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H149" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3537,7 +3477,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="8:9">
+    <row r="150" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H150" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3547,7 +3487,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="8:9">
+    <row r="151" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H151" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3557,7 +3497,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="8:9">
+    <row r="152" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H152" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3567,7 +3507,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="8:9">
+    <row r="153" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H153" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3577,7 +3517,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="8:9">
+    <row r="154" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H154" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3587,7 +3527,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="8:9">
+    <row r="155" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H155" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3597,7 +3537,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="8:9">
+    <row r="156" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H156" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3607,7 +3547,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="8:9">
+    <row r="157" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H157" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3617,7 +3557,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="8:9">
+    <row r="158" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H158" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3627,7 +3567,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="8:9">
+    <row r="159" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H159" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3637,7 +3577,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="8:9">
+    <row r="160" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H160" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3647,7 +3587,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="8:9">
+    <row r="161" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H161" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3657,7 +3597,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="8:9">
+    <row r="162" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H162" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3667,7 +3607,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="8:9">
+    <row r="163" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H163" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3677,7 +3617,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="8:9">
+    <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3687,7 +3627,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="8:9">
+    <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3697,7 +3637,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="8:9">
+    <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3707,7 +3647,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="8:9">
+    <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3717,7 +3657,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="8:9">
+    <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3727,7 +3667,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="8:9">
+    <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3737,7 +3677,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="8:9">
+    <row r="170" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H170" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3747,7 +3687,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="8:9">
+    <row r="171" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H171" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3757,7 +3697,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="8:9">
+    <row r="172" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H172" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3767,7 +3707,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="8:9">
+    <row r="173" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H173" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3777,7 +3717,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="8:9">
+    <row r="174" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H174" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3787,7 +3727,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="8:9">
+    <row r="175" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H175" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3797,7 +3737,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="8:9">
+    <row r="176" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H176" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3807,7 +3747,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="8:9">
+    <row r="177" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H177" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3817,7 +3757,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="8:9">
+    <row r="178" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H178" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3827,7 +3767,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="8:9">
+    <row r="179" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H179" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3837,7 +3777,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="8:9">
+    <row r="180" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H180" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3847,7 +3787,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="8:9">
+    <row r="181" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H181" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3857,7 +3797,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="8:9">
+    <row r="182" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H182" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3867,7 +3807,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="8:9">
+    <row r="183" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H183" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3877,7 +3817,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="8:9">
+    <row r="184" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H184" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3887,7 +3827,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="8:9">
+    <row r="185" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H185" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3897,7 +3837,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="8:9">
+    <row r="186" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H186" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3907,7 +3847,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="8:9">
+    <row r="187" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H187" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3917,7 +3857,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="8:9">
+    <row r="188" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H188" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3927,7 +3867,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="8:9">
+    <row r="189" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H189" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3937,7 +3877,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="8:9">
+    <row r="190" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H190" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3947,7 +3887,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="8:9">
+    <row r="191" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H191" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3957,7 +3897,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="8:9">
+    <row r="192" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H192" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3967,7 +3907,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="8:9">
+    <row r="193" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H193" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3977,7 +3917,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="8:9">
+    <row r="194" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H194" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3987,7 +3927,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="8:9">
+    <row r="195" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H195" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3997,7 +3937,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="8:9">
+    <row r="196" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H196" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4007,7 +3947,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="8:9">
+    <row r="197" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H197" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4017,7 +3957,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="8:9">
+    <row r="198" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H198" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4027,7 +3967,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="8:9">
+    <row r="199" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H199" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4037,7 +3977,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="8:9">
+    <row r="200" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H200" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4047,7 +3987,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="8:9">
+    <row r="201" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H201" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4057,7 +3997,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="8:9">
+    <row r="202" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H202" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4067,7 +4007,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="8:9">
+    <row r="203" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H203" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4077,7 +4017,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="8:9">
+    <row r="204" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H204" s="12" t="str">
         <f t="shared" ref="H204:H231" si="6">IF(OR(D204="", E204=""), "", D204-E204)</f>
         <v/>
@@ -4087,7 +4027,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="8:9">
+    <row r="205" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H205" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4097,7 +4037,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="8:9">
+    <row r="206" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H206" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4107,7 +4047,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="8:9">
+    <row r="207" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H207" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4117,7 +4057,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="8:9">
+    <row r="208" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H208" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4127,7 +4067,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="8:9">
+    <row r="209" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H209" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4137,7 +4077,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="8:9">
+    <row r="210" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H210" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4147,7 +4087,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="8:9">
+    <row r="211" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H211" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4157,7 +4097,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="8:9">
+    <row r="212" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H212" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4167,7 +4107,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="8:9">
+    <row r="213" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H213" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4177,7 +4117,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="8:9">
+    <row r="214" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H214" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4187,7 +4127,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="8:9">
+    <row r="215" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H215" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4197,7 +4137,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="8:9">
+    <row r="216" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H216" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4207,7 +4147,7 @@
         <v/>
       </c>
     </row>
-    <row r="217" spans="8:9">
+    <row r="217" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H217" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4217,7 +4157,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="8:9">
+    <row r="218" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H218" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4227,7 +4167,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="8:9">
+    <row r="219" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H219" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4237,7 +4177,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="8:9">
+    <row r="220" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H220" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4247,7 +4187,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="8:9">
+    <row r="221" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H221" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4257,7 +4197,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="8:9">
+    <row r="222" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H222" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4267,7 +4207,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="8:9">
+    <row r="223" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H223" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4277,7 +4217,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="8:9">
+    <row r="224" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H224" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4287,7 +4227,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="8:9">
+    <row r="225" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H225" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4297,7 +4237,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="8:9">
+    <row r="226" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H226" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4307,7 +4247,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="8:9">
+    <row r="227" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H227" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4317,7 +4257,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="8:9">
+    <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H228" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4327,7 +4267,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="8:9">
+    <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H229" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4337,7 +4277,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="8:9">
+    <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H230" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4347,7 +4287,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="8:9">
+    <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H231" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4357,43 +4297,43 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="8:9">
+    <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I232" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="233" spans="8:9">
+    <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I233" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="234" spans="8:9">
+    <row r="234" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I234" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="235" spans="8:9">
+    <row r="235" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I235" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="8:9">
+    <row r="236" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I236" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="8:9">
+    <row r="237" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I237" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="8:9">
+    <row r="238" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I238" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -4401,40 +4341,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="F34:F43 F45:F65518 F5:F23 F25:F32">
-    <cfRule type="cellIs" dxfId="11" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"Delayed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="32" stopIfTrue="1" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="33" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="8" priority="28" stopIfTrue="1" operator="equal">
-      <formula>"Delayed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="29" stopIfTrue="1" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="30" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
-    <cfRule type="cellIs" dxfId="5" priority="25" stopIfTrue="1" operator="equal">
-      <formula>"Delayed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
+  <conditionalFormatting sqref="F5:F65518">
     <cfRule type="cellIs" dxfId="2" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Delayed"</formula>
     </cfRule>

</xml_diff>